<commit_message>
Produced alignment plots of primer regions
</commit_message>
<xml_diff>
--- a/sample_info/Botrytis_isolates_for_WGS_CAGRF20074.xlsx
+++ b/sample_info/Botrytis_isolates_for_WGS_CAGRF20074.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://griffitheduau-my.sharepoint.com/personal/i_bar_griffith_edu_au/Documents/Research/A_rabiei/B_cinerea_WGS/B_cinerea_probe_alignment/sample_info/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ido Bar\OneDrive - Griffith University\Research\A_rabiei\B_cinerea_WGS\B_cinerea_probe_alignment\sample_info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{41DEBC4C-6AED-4FCC-88AD-0E44493EDA63}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{41DEBC4C-6AED-4FCC-88AD-0E44493EDA63}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{F845305D-6117-48FF-971D-E48A701B54F3}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{DBA59634-1BD7-4666-AA30-C7F064329A43}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="13096" xr2:uid="{DBA59634-1BD7-4666-AA30-C7F064329A43}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -69,7 +69,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Ford lab:</t>
         </r>
@@ -78,7 +78,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 B. fabae samples</t>
@@ -150,7 +150,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -178,19 +178,6 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -585,12 +572,13 @@
       <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
+    <col min="3" max="3" width="12.796875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -604,7 +592,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -618,7 +606,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -632,7 +620,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -646,7 +634,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -660,7 +648,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -674,7 +662,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -688,7 +676,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -702,7 +690,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -716,7 +704,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -730,7 +718,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -744,7 +732,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -758,7 +746,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -772,7 +760,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -786,7 +774,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -800,7 +788,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -814,7 +802,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -828,7 +816,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -842,7 +830,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19" s="5">
         <v>18</v>
       </c>
@@ -856,7 +844,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -870,7 +858,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -884,7 +872,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -898,7 +886,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A23" s="5">
         <v>22</v>
       </c>
@@ -919,6 +907,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010038EC5152544FA941B2FCF6FC911C1211" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7c65ce02839d668ca9eba218866de938">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="f38ef60c-44b8-4b3e-b84e-3f774f47ec01" xmlns:ns4="77420ce7-ad61-40a5-b28d-42d2f2a680a0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f5d8e21d1066e7b0b912dd2073999255" ns3:_="" ns4:_="">
     <xsd:import namespace="f38ef60c-44b8-4b3e-b84e-3f774f47ec01"/>
@@ -1127,15 +1124,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1143,6 +1131,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{63032345-89F1-43C5-B3F0-63B20129D32D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5112FC15-3CBE-43DE-AC8F-036D04ED76AE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1161,27 +1157,19 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{63032345-89F1-43C5-B3F0-63B20129D32D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{47C9BC18-B232-4556-B2AB-23A418B623E1}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="f38ef60c-44b8-4b3e-b84e-3f774f47ec01"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="77420ce7-ad61-40a5-b28d-42d2f2a680a0"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="f38ef60c-44b8-4b3e-b84e-3f774f47ec01"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>